<commit_message>
modificacion de matriz de riesgos version 1.1
</commit_message>
<xml_diff>
--- a/9°A/administracion_proyectos/Unidad 3/U3-APTI2-Rúbricas/Matriz de riesgos completa.xlsx
+++ b/9°A/administracion_proyectos/Unidad 3/U3-APTI2-Rúbricas/Matriz de riesgos completa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unidad 3\U3-APTI2-Rúbricas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecy Tapia\Desktop\SM-ROOT\9°A\administracion_proyectos\Unidad 3\U3-APTI2-Rúbricas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -1524,67 +1524,67 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1946,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2707,18 +2707,18 @@
     </row>
     <row r="3" spans="2:17" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="149"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
       <c r="M3" s="14"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
@@ -2754,10 +2754,10 @@
       <c r="I5" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="150" t="s">
+      <c r="J5" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="150"/>
+      <c r="K5" s="135"/>
       <c r="L5" s="39" t="s">
         <v>36</v>
       </c>
@@ -2782,10 +2782,10 @@
       <c r="I6" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="151" t="s">
+      <c r="J6" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="151"/>
+      <c r="K6" s="136"/>
       <c r="L6" s="42">
         <f>16/25*100</f>
         <v>64</v>
@@ -2811,10 +2811,10 @@
       <c r="I7" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="145" t="s">
+      <c r="J7" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="145"/>
+      <c r="K7" s="137"/>
       <c r="L7" s="47">
         <f>15/25*100</f>
         <v>60</v>
@@ -2840,10 +2840,10 @@
       <c r="I8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="145" t="s">
+      <c r="J8" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="145"/>
+      <c r="K8" s="137"/>
       <c r="L8" s="47">
         <f>12/25*100</f>
         <v>48</v>
@@ -2869,10 +2869,10 @@
       <c r="I9" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="145" t="s">
+      <c r="J9" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="145"/>
+      <c r="K9" s="137"/>
       <c r="L9" s="47">
         <f>8/25*100</f>
         <v>32</v>
@@ -2898,10 +2898,10 @@
       <c r="I10" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="146" t="s">
+      <c r="J10" s="138" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="146"/>
+      <c r="K10" s="138"/>
       <c r="L10" s="52">
         <f>5/25*100</f>
         <v>20</v>
@@ -2947,10 +2947,10 @@
       <c r="C13" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="147" t="s">
+      <c r="D13" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="147"/>
+      <c r="E13" s="139"/>
       <c r="F13" s="56" t="s">
         <v>54</v>
       </c>
@@ -2980,11 +2980,11 @@
         <f>CONCATENATE($B$13,Matriz!B16)</f>
         <v>R1</v>
       </c>
-      <c r="D14" s="148" t="str">
+      <c r="D14" s="140" t="str">
         <f>Matriz!E16</f>
         <v>Desconocimiento del proceso</v>
       </c>
-      <c r="E14" s="148"/>
+      <c r="E14" s="140"/>
       <c r="F14" s="59" t="str">
         <f>Matriz!F16</f>
         <v>Personal nuevo</v>
@@ -3624,11 +3624,11 @@
         <f t="shared" ref="C33:D47" si="3">C14</f>
         <v>R1</v>
       </c>
-      <c r="D33" s="138" t="str">
+      <c r="D33" s="145" t="str">
         <f t="shared" si="3"/>
         <v>Desconocimiento del proceso</v>
       </c>
-      <c r="E33" s="138"/>
+      <c r="E33" s="145"/>
       <c r="F33" s="71" t="str">
         <f t="shared" ref="F33:F47" si="4">K14</f>
         <v>MODERADO</v>
@@ -3646,11 +3646,11 @@
       <c r="J33" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="K33" s="139" t="str">
+      <c r="K33" s="146" t="str">
         <f>Matriz!K16</f>
         <v>Verificar la instalación electrica del local y utilizar no breaks</v>
       </c>
-      <c r="L33" s="139"/>
+      <c r="L33" s="146"/>
       <c r="M33" s="14"/>
     </row>
     <row r="34" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3659,11 +3659,11 @@
         <f t="shared" si="3"/>
         <v>R2</v>
       </c>
-      <c r="D34" s="140" t="str">
+      <c r="D34" s="147" t="str">
         <f t="shared" si="3"/>
         <v>Falta precisión</v>
       </c>
-      <c r="E34" s="140"/>
+      <c r="E34" s="147"/>
       <c r="F34" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3677,11 +3677,11 @@
         <v>67</v>
       </c>
       <c r="J34" s="74"/>
-      <c r="K34" s="137">
+      <c r="K34" s="148">
         <f>Matriz!K17</f>
         <v>0</v>
       </c>
-      <c r="L34" s="137"/>
+      <c r="L34" s="148"/>
       <c r="M34" s="14"/>
     </row>
     <row r="35" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3690,11 +3690,11 @@
         <f t="shared" si="3"/>
         <v>R3</v>
       </c>
-      <c r="D35" s="136" t="str">
+      <c r="D35" s="149" t="str">
         <f t="shared" si="3"/>
         <v>Demora en solicitar</v>
       </c>
-      <c r="E35" s="136"/>
+      <c r="E35" s="149"/>
       <c r="F35" s="76" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3708,11 +3708,11 @@
         <v>67</v>
       </c>
       <c r="J35" s="75"/>
-      <c r="K35" s="137">
+      <c r="K35" s="148">
         <f>Matriz!K18</f>
         <v>0</v>
       </c>
-      <c r="L35" s="137"/>
+      <c r="L35" s="148"/>
       <c r="M35" s="14"/>
     </row>
     <row r="36" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3721,11 +3721,11 @@
         <f t="shared" si="3"/>
         <v>R4</v>
       </c>
-      <c r="D36" s="136" t="str">
+      <c r="D36" s="149" t="str">
         <f t="shared" si="3"/>
         <v>Demora en reportes</v>
       </c>
-      <c r="E36" s="136"/>
+      <c r="E36" s="149"/>
       <c r="F36" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3739,11 +3739,11 @@
         <v>67</v>
       </c>
       <c r="J36" s="74"/>
-      <c r="K36" s="137">
+      <c r="K36" s="148">
         <f>Matriz!K19</f>
         <v>0</v>
       </c>
-      <c r="L36" s="137"/>
+      <c r="L36" s="148"/>
       <c r="M36" s="14"/>
     </row>
     <row r="37" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3752,11 +3752,11 @@
         <f t="shared" si="3"/>
         <v>R5</v>
       </c>
-      <c r="D37" s="136" t="str">
+      <c r="D37" s="149" t="str">
         <f t="shared" si="3"/>
         <v>Uso inadecuado de programas</v>
       </c>
-      <c r="E37" s="136"/>
+      <c r="E37" s="149"/>
       <c r="F37" s="76" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3770,11 +3770,11 @@
         <v>67</v>
       </c>
       <c r="J37" s="75"/>
-      <c r="K37" s="137">
+      <c r="K37" s="148">
         <f>Matriz!K20</f>
         <v>0</v>
       </c>
-      <c r="L37" s="137"/>
+      <c r="L37" s="148"/>
       <c r="M37" s="14"/>
     </row>
     <row r="38" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3783,11 +3783,11 @@
         <f t="shared" si="3"/>
         <v>R6</v>
       </c>
-      <c r="D38" s="134">
+      <c r="D38" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E38" s="134"/>
+      <c r="E38" s="150"/>
       <c r="F38" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3801,11 +3801,11 @@
         <v>67</v>
       </c>
       <c r="J38" s="79"/>
-      <c r="K38" s="135">
+      <c r="K38" s="151">
         <f>Matriz!K21</f>
         <v>0</v>
       </c>
-      <c r="L38" s="135"/>
+      <c r="L38" s="151"/>
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3814,11 +3814,11 @@
         <f t="shared" si="3"/>
         <v>R7</v>
       </c>
-      <c r="D39" s="134">
+      <c r="D39" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E39" s="134"/>
+      <c r="E39" s="150"/>
       <c r="F39" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3832,11 +3832,11 @@
         <v>67</v>
       </c>
       <c r="J39" s="79"/>
-      <c r="K39" s="135">
+      <c r="K39" s="151">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="L39" s="135"/>
+      <c r="L39" s="151"/>
       <c r="M39" s="14"/>
     </row>
     <row r="40" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3845,11 +3845,11 @@
         <f t="shared" si="3"/>
         <v>R8</v>
       </c>
-      <c r="D40" s="134">
+      <c r="D40" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E40" s="134"/>
+      <c r="E40" s="150"/>
       <c r="F40" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3863,11 +3863,11 @@
         <v>67</v>
       </c>
       <c r="J40" s="79"/>
-      <c r="K40" s="135">
+      <c r="K40" s="151">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="L40" s="135"/>
+      <c r="L40" s="151"/>
       <c r="M40" s="14"/>
     </row>
     <row r="41" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3876,11 +3876,11 @@
         <f t="shared" si="3"/>
         <v>R9</v>
       </c>
-      <c r="D41" s="134">
+      <c r="D41" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E41" s="134"/>
+      <c r="E41" s="150"/>
       <c r="F41" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3894,11 +3894,11 @@
         <v>67</v>
       </c>
       <c r="J41" s="79"/>
-      <c r="K41" s="135">
+      <c r="K41" s="151">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="L41" s="135"/>
+      <c r="L41" s="151"/>
       <c r="M41" s="14"/>
     </row>
     <row r="42" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3907,11 +3907,11 @@
         <f t="shared" si="3"/>
         <v>R10</v>
       </c>
-      <c r="D42" s="134">
+      <c r="D42" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E42" s="134"/>
+      <c r="E42" s="150"/>
       <c r="F42" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3925,11 +3925,11 @@
         <v>67</v>
       </c>
       <c r="J42" s="79"/>
-      <c r="K42" s="135">
+      <c r="K42" s="151">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="L42" s="135"/>
+      <c r="L42" s="151"/>
       <c r="M42" s="14"/>
     </row>
     <row r="43" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3938,11 +3938,11 @@
         <f t="shared" si="3"/>
         <v>R11</v>
       </c>
-      <c r="D43" s="134">
+      <c r="D43" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E43" s="134"/>
+      <c r="E43" s="150"/>
       <c r="F43" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3956,11 +3956,11 @@
         <v>67</v>
       </c>
       <c r="J43" s="79"/>
-      <c r="K43" s="135">
+      <c r="K43" s="151">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="L43" s="135"/>
+      <c r="L43" s="151"/>
       <c r="M43" s="14"/>
     </row>
     <row r="44" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3969,11 +3969,11 @@
         <f t="shared" si="3"/>
         <v>R12</v>
       </c>
-      <c r="D44" s="134">
+      <c r="D44" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E44" s="134"/>
+      <c r="E44" s="150"/>
       <c r="F44" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3987,11 +3987,11 @@
         <v>67</v>
       </c>
       <c r="J44" s="79"/>
-      <c r="K44" s="135">
+      <c r="K44" s="151">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="L44" s="135"/>
+      <c r="L44" s="151"/>
       <c r="M44" s="14"/>
     </row>
     <row r="45" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4000,11 +4000,11 @@
         <f t="shared" si="3"/>
         <v>R13</v>
       </c>
-      <c r="D45" s="134">
+      <c r="D45" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E45" s="134"/>
+      <c r="E45" s="150"/>
       <c r="F45" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4018,11 +4018,11 @@
         <v>67</v>
       </c>
       <c r="J45" s="79"/>
-      <c r="K45" s="135">
+      <c r="K45" s="151">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="L45" s="135"/>
+      <c r="L45" s="151"/>
       <c r="M45" s="14"/>
     </row>
     <row r="46" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4031,11 +4031,11 @@
         <f t="shared" si="3"/>
         <v>R14</v>
       </c>
-      <c r="D46" s="134">
+      <c r="D46" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E46" s="134"/>
+      <c r="E46" s="150"/>
       <c r="F46" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4049,11 +4049,11 @@
         <v>67</v>
       </c>
       <c r="J46" s="79"/>
-      <c r="K46" s="135">
+      <c r="K46" s="151">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="L46" s="135"/>
+      <c r="L46" s="151"/>
       <c r="M46" s="14"/>
     </row>
     <row r="47" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4062,11 +4062,11 @@
         <f t="shared" si="3"/>
         <v>R15</v>
       </c>
-      <c r="D47" s="134">
+      <c r="D47" s="150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E47" s="134"/>
+      <c r="E47" s="150"/>
       <c r="F47" s="78" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4080,11 +4080,11 @@
         <v>67</v>
       </c>
       <c r="J47" s="79"/>
-      <c r="K47" s="135">
+      <c r="K47" s="151">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="L47" s="135"/>
+      <c r="L47" s="151"/>
       <c r="M47" s="14"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
@@ -4131,62 +4131,62 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="K35:L35"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="K32:L32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="L14:L28">
     <cfRule type="colorScale" priority="2">
@@ -4240,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8:N8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4256,21 +4256,21 @@
   <sheetData>
     <row r="4" spans="3:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="152" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="153"/>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="153"/>
-      <c r="L5" s="153"/>
-      <c r="M5" s="153"/>
-      <c r="N5" s="153"/>
-      <c r="O5" s="153"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
+      <c r="J5" s="152"/>
+      <c r="K5" s="152"/>
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="152"/>
+      <c r="O5" s="152"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="12"/>
@@ -4292,10 +4292,10 @@
       <c r="D7" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="154" t="s">
+      <c r="E7" s="153" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="154"/>
+      <c r="F7" s="153"/>
       <c r="G7" s="83" t="s">
         <v>62</v>
       </c>
@@ -4314,10 +4314,10 @@
       <c r="L7" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="154" t="s">
+      <c r="M7" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="154"/>
+      <c r="N7" s="153"/>
       <c r="O7" s="14"/>
     </row>
     <row r="8" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4326,11 +4326,11 @@
         <f>'Cualitativo y Cuantitativo'!C33</f>
         <v>R1</v>
       </c>
-      <c r="E8" s="152" t="str">
+      <c r="E8" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D33</f>
         <v>Desconocimiento del proceso</v>
       </c>
-      <c r="F8" s="152"/>
+      <c r="F8" s="154"/>
       <c r="G8" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F33</f>
         <v>MODERADO</v>
@@ -4353,8 +4353,8 @@
         <f>'Cualitativo y Cuantitativo'!J33</f>
         <v>Project Manager</v>
       </c>
-      <c r="M8" s="152"/>
-      <c r="N8" s="152"/>
+      <c r="M8" s="154"/>
+      <c r="N8" s="154"/>
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4363,11 +4363,11 @@
         <f>'Cualitativo y Cuantitativo'!C34</f>
         <v>R2</v>
       </c>
-      <c r="E9" s="152" t="str">
+      <c r="E9" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D34</f>
         <v>Falta precisión</v>
       </c>
-      <c r="F9" s="152"/>
+      <c r="F9" s="154"/>
       <c r="G9" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F34</f>
         <v>MUY BAJO</v>
@@ -4386,8 +4386,8 @@
         <f>'Cualitativo y Cuantitativo'!J34</f>
         <v>0</v>
       </c>
-      <c r="M9" s="152"/>
-      <c r="N9" s="152"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4396,11 +4396,11 @@
         <f>'Cualitativo y Cuantitativo'!C35</f>
         <v>R3</v>
       </c>
-      <c r="E10" s="152" t="str">
+      <c r="E10" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D35</f>
         <v>Demora en solicitar</v>
       </c>
-      <c r="F10" s="152"/>
+      <c r="F10" s="154"/>
       <c r="G10" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F35</f>
         <v>MUY BAJO</v>
@@ -4419,8 +4419,8 @@
         <f>'Cualitativo y Cuantitativo'!J35</f>
         <v>0</v>
       </c>
-      <c r="M10" s="152"/>
-      <c r="N10" s="152"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="154"/>
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4429,11 +4429,11 @@
         <f>'Cualitativo y Cuantitativo'!C36</f>
         <v>R4</v>
       </c>
-      <c r="E11" s="152" t="str">
+      <c r="E11" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D36</f>
         <v>Demora en reportes</v>
       </c>
-      <c r="F11" s="152"/>
+      <c r="F11" s="154"/>
       <c r="G11" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F36</f>
         <v>MUY BAJO</v>
@@ -4452,8 +4452,8 @@
         <f>'Cualitativo y Cuantitativo'!J36</f>
         <v>0</v>
       </c>
-      <c r="M11" s="152"/>
-      <c r="N11" s="152"/>
+      <c r="M11" s="154"/>
+      <c r="N11" s="154"/>
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4462,11 +4462,11 @@
         <f>'Cualitativo y Cuantitativo'!C37</f>
         <v>R5</v>
       </c>
-      <c r="E12" s="152" t="str">
+      <c r="E12" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D37</f>
         <v>Uso inadecuado de programas</v>
       </c>
-      <c r="F12" s="152"/>
+      <c r="F12" s="154"/>
       <c r="G12" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F37</f>
         <v>MUY BAJO</v>
@@ -4485,8 +4485,8 @@
         <f>'Cualitativo y Cuantitativo'!J37</f>
         <v>0</v>
       </c>
-      <c r="M12" s="152"/>
-      <c r="N12" s="152"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="154"/>
       <c r="O12" s="14"/>
     </row>
     <row r="13" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4495,11 +4495,11 @@
         <f>'Cualitativo y Cuantitativo'!C38</f>
         <v>R6</v>
       </c>
-      <c r="E13" s="152">
+      <c r="E13" s="154">
         <f>'Cualitativo y Cuantitativo'!D38</f>
         <v>0</v>
       </c>
-      <c r="F13" s="152"/>
+      <c r="F13" s="154"/>
       <c r="G13" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F38</f>
         <v>MUY BAJO</v>
@@ -4518,8 +4518,8 @@
         <f>'Cualitativo y Cuantitativo'!J38</f>
         <v>0</v>
       </c>
-      <c r="M13" s="152"/>
-      <c r="N13" s="152"/>
+      <c r="M13" s="154"/>
+      <c r="N13" s="154"/>
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4528,11 +4528,11 @@
         <f>'Cualitativo y Cuantitativo'!C39</f>
         <v>R7</v>
       </c>
-      <c r="E14" s="152">
+      <c r="E14" s="154">
         <f>'Cualitativo y Cuantitativo'!D39</f>
         <v>0</v>
       </c>
-      <c r="F14" s="152"/>
+      <c r="F14" s="154"/>
       <c r="G14" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F39</f>
         <v>MUY BAJO</v>
@@ -4551,8 +4551,8 @@
         <f>'Cualitativo y Cuantitativo'!J39</f>
         <v>0</v>
       </c>
-      <c r="M14" s="152"/>
-      <c r="N14" s="152"/>
+      <c r="M14" s="154"/>
+      <c r="N14" s="154"/>
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4561,11 +4561,11 @@
         <f>'Cualitativo y Cuantitativo'!C40</f>
         <v>R8</v>
       </c>
-      <c r="E15" s="152">
+      <c r="E15" s="154">
         <f>'Cualitativo y Cuantitativo'!D40</f>
         <v>0</v>
       </c>
-      <c r="F15" s="152"/>
+      <c r="F15" s="154"/>
       <c r="G15" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F40</f>
         <v>MUY BAJO</v>
@@ -4584,8 +4584,8 @@
         <f>'Cualitativo y Cuantitativo'!J40</f>
         <v>0</v>
       </c>
-      <c r="M15" s="152"/>
-      <c r="N15" s="152"/>
+      <c r="M15" s="154"/>
+      <c r="N15" s="154"/>
       <c r="O15" s="14"/>
     </row>
     <row r="16" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4594,11 +4594,11 @@
         <f>'Cualitativo y Cuantitativo'!C41</f>
         <v>R9</v>
       </c>
-      <c r="E16" s="152">
+      <c r="E16" s="154">
         <f>'Cualitativo y Cuantitativo'!D41</f>
         <v>0</v>
       </c>
-      <c r="F16" s="152"/>
+      <c r="F16" s="154"/>
       <c r="G16" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F41</f>
         <v>MUY BAJO</v>
@@ -4617,8 +4617,8 @@
         <f>'Cualitativo y Cuantitativo'!J41</f>
         <v>0</v>
       </c>
-      <c r="M16" s="152"/>
-      <c r="N16" s="152"/>
+      <c r="M16" s="154"/>
+      <c r="N16" s="154"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4627,11 +4627,11 @@
         <f>'Cualitativo y Cuantitativo'!C42</f>
         <v>R10</v>
       </c>
-      <c r="E17" s="152">
+      <c r="E17" s="154">
         <f>'Cualitativo y Cuantitativo'!D42</f>
         <v>0</v>
       </c>
-      <c r="F17" s="152"/>
+      <c r="F17" s="154"/>
       <c r="G17" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F42</f>
         <v>MUY BAJO</v>
@@ -4650,8 +4650,8 @@
         <f>'Cualitativo y Cuantitativo'!J42</f>
         <v>0</v>
       </c>
-      <c r="M17" s="152"/>
-      <c r="N17" s="152"/>
+      <c r="M17" s="154"/>
+      <c r="N17" s="154"/>
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4660,11 +4660,11 @@
         <f>'Cualitativo y Cuantitativo'!C43</f>
         <v>R11</v>
       </c>
-      <c r="E18" s="152">
+      <c r="E18" s="154">
         <f>'Cualitativo y Cuantitativo'!D43</f>
         <v>0</v>
       </c>
-      <c r="F18" s="152"/>
+      <c r="F18" s="154"/>
       <c r="G18" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F43</f>
         <v>MUY BAJO</v>
@@ -4683,8 +4683,8 @@
         <f>'Cualitativo y Cuantitativo'!J43</f>
         <v>0</v>
       </c>
-      <c r="M18" s="152"/>
-      <c r="N18" s="152"/>
+      <c r="M18" s="154"/>
+      <c r="N18" s="154"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4693,11 +4693,11 @@
         <f>'Cualitativo y Cuantitativo'!C44</f>
         <v>R12</v>
       </c>
-      <c r="E19" s="152">
+      <c r="E19" s="154">
         <f>'Cualitativo y Cuantitativo'!D44</f>
         <v>0</v>
       </c>
-      <c r="F19" s="152"/>
+      <c r="F19" s="154"/>
       <c r="G19" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F44</f>
         <v>MUY BAJO</v>
@@ -4716,8 +4716,8 @@
         <f>'Cualitativo y Cuantitativo'!J44</f>
         <v>0</v>
       </c>
-      <c r="M19" s="152"/>
-      <c r="N19" s="152"/>
+      <c r="M19" s="154"/>
+      <c r="N19" s="154"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4726,11 +4726,11 @@
         <f>'Cualitativo y Cuantitativo'!C45</f>
         <v>R13</v>
       </c>
-      <c r="E20" s="152">
+      <c r="E20" s="154">
         <f>'Cualitativo y Cuantitativo'!D45</f>
         <v>0</v>
       </c>
-      <c r="F20" s="152"/>
+      <c r="F20" s="154"/>
       <c r="G20" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F45</f>
         <v>MUY BAJO</v>
@@ -4749,8 +4749,8 @@
         <f>'Cualitativo y Cuantitativo'!J45</f>
         <v>0</v>
       </c>
-      <c r="M20" s="152"/>
-      <c r="N20" s="152"/>
+      <c r="M20" s="154"/>
+      <c r="N20" s="154"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4759,11 +4759,11 @@
         <f>'Cualitativo y Cuantitativo'!C46</f>
         <v>R14</v>
       </c>
-      <c r="E21" s="152">
+      <c r="E21" s="154">
         <f>'Cualitativo y Cuantitativo'!D46</f>
         <v>0</v>
       </c>
-      <c r="F21" s="152"/>
+      <c r="F21" s="154"/>
       <c r="G21" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F46</f>
         <v>MUY BAJO</v>
@@ -4782,8 +4782,8 @@
         <f>'Cualitativo y Cuantitativo'!J46</f>
         <v>0</v>
       </c>
-      <c r="M21" s="152"/>
-      <c r="N21" s="152"/>
+      <c r="M21" s="154"/>
+      <c r="N21" s="154"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -4792,11 +4792,11 @@
         <f>'Cualitativo y Cuantitativo'!C47</f>
         <v>R15</v>
       </c>
-      <c r="E22" s="152">
+      <c r="E22" s="154">
         <f>'Cualitativo y Cuantitativo'!D47</f>
         <v>0</v>
       </c>
-      <c r="F22" s="152"/>
+      <c r="F22" s="154"/>
       <c r="G22" s="86" t="str">
         <f>'Cualitativo y Cuantitativo'!F47</f>
         <v>MUY BAJO</v>
@@ -4815,8 +4815,8 @@
         <f>'Cualitativo y Cuantitativo'!J47</f>
         <v>0</v>
       </c>
-      <c r="M22" s="152"/>
-      <c r="N22" s="152"/>
+      <c r="M22" s="154"/>
+      <c r="N22" s="154"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.2">
@@ -4866,29 +4866,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C5:O5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M17:N17"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E22:F22"/>
@@ -4899,6 +4876,29 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="C5:O5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>